<commit_message>
Next steps (Store the selected_answer and give the score)
</commit_message>
<xml_diff>
--- a/generated_questions.xlsx
+++ b/generated_questions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,177 +436,302 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>question</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>context</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>options</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>option1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>option2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>correct_answer</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>used</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>What is the name of the Amazon Rainfo rest?</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>TheAmazonRainforest,oftenreferredtoasthe"lungsoftheEarth,"playsacrucialroleinregulating theplanet'soxygenandcarbondioxidelevels.Coveringanareaofapproximately5.5millionsquare kilometers,theforestspansacrossninecountriesinSouthAmerica,withthemajoritylocatedinBrazil.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>['TheAmazonRainforest', 'adolescent']</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>TheAmazonRainforest</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>adolescent</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TheAmazonRainforest</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>What is home to an astonishing diversity of wild life?</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Itishometoanastonishingdiversityofwildlife,includingjaguars,sloths,andmorethan2.5million speciesofinsects.Despiteitsimportance,theAmazonfacessignificantthreatsduetodeforestation, illegallogging,andagriculturalexpansion.Scientistswarnthatcontinueddestructioncouldleadto irreversibledamage,affectingnotonlylocalecosystemsbutalsoglobalclimatepatterns.TheAmazon alsoplaysavitalroleinthewatercycle,generatingrainthatsustainsagricultureinnearbyregions.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>['Itishometoanastonishingdiversityofwildlife', 'a sand castle']</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Itishometoanastonishingdiversityofwildlife</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>a sand castle</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Itishometoanastonishingdiversityofwildlife</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>What are indigenous communities relying on?</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Indigenouscommunitieshavelivedintheforestforthousandsofyears,relyingonitsresourcesfor food,shelter,andmedicine.EffortstoprotecttheAmazonincludeinternationalagreementsand conservationprojects,butenforcementremainsachallenge.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>['relyingonitsresourcesfor food,shelter,andmedicine', 'a sandstone']</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>relyingonitsresourcesfor food,shelter,andmedicine</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>a sandstone</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>relyingonitsresourcesfor food,shelter,andmedicine</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>What was the discovery of penicillin by Alexander Fleming in 1928?</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>ThediscoveryofpenicillinbyAlexanderFlemingin1928markedthebeginningofthemodernantibiotic era.Penicillin,amold-derivedantibiotic,wasfoundtoeffectivelykillawiderangeofbacterial infections,revolutionizingmedicine.Beforeitswidespreaduse,evenminorinjuriesorcommon illnesseslikepneumoniacouldbefatalduetotheriskofinfection.DuringWorldWarII,penicillinwas mass-producedandusedextensivelytotreatwoundedsoldiers,savingcountlesslives.Fleming's discoveryearnedhimtheNobelPrizeinPhysiologyorMedicinein1945,sharedwithHowardFlorey andErnstBorisChain,whoplayedcrucialrolesindevelopingpenicillinformedicaluse.However,over time,theoveruseandmisuseofantibioticshaveledtotheemergenceofantibiotic-resistantbacteria, posinganewchallengetomodernhealthcare.Today,researcherscontinuetoseeknewwaysto combattheseresistantstrainswhilepromotingresponsibleuseofantibiotics.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>['discoveryearnedhimtheNobelPrizeinPhysiologyorMedicinein1945', 'a syringe']</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>discoveryearnedhimtheNobelPrizeinPhysiologyorMedicinein1945</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>a syringe</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>discoveryearnedhimtheNobelPrizeinPhysiologyorMedicinein1945</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>What is the reason for the rise of social media?</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>TheInternethastransformedthewaypeoplecommunicate,work,andaccessinformation.Sinceits inceptioninthelate20thcentury,theInternethasgrownexponentially,connectingbillionsofusers worldwide.Itallowsfortheinstanttransmissionofdata,whetherthroughemails,socialmedia,or videocalls,makingglobalcommunicationmoreaccessiblethaneverbefore.E-commercehasalso flourished,enablingconsumerstoshoponlineandhavegoodsdeliveredtotheirdoorsteps.In education,theInternethasopenedupopportunitiesforonlinelearning,withcountlessresources availableattheclickofabutton.Despitethesebenefits,theInternethasalsobroughtchallenges,such asprivacyconcerns,thespreadofmisinformation,andcybercrime.Theriseofsocialmediahas changedthedynamicsofhumaninteraction,withbothpositiveandnegativeimpactsonmentalhealth.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>['E-commercehasalso flourished', 'a lot of people are a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a']</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>E-commercehasalso flourished</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>a lot of people are a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a lot more likely to be a</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>E-commercehasalso flourished</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>What is the main reason for governments and organizations to grow?</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Governmentsandorganizationscontinuetograpplewithhowtoregulatethedigitalspacewhile preservingfreedomofexpressionandinnovation.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>['preservingfreedomofexpressionandinnovation', 'a new generation']</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>preservingfreedomofexpressionandinnovation</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>a new generation</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>preservingfreedomofexpressionandinnovation</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>What is the most pressing issues facing humanity today?</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Climatechangeisoneofthemostpressingissuesfacinghumanitytoday.Drivenlargelybyhuman activitiessuchasburningfossilfuels,deforestation,andindustrialprocesses,theEarth'saverage temperaturehasbeenrisingatanunprecedentedrate.Thisincreaseintemperaturehasledtomore frequentandsevereweatherevents,includinghurricanes,floods,anddroughts.Polaricecapsand glaciersaremelting,contributingtorisingsealevelsthatthreatencoastalcommunitiesworldwide.In additiontoenvironmentalimpacts,climatechangeisalsoaffectingglobalfoodsecurity,aschanging weatherpatternsdisruptagriculture.Scientistsagreethaturgentactionisneededtoreduce greenhousegasemissionsandtransitiontomoresustainableenergysourceslikewindandsolarpower.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>includinghurricanes,floods,anddroughts</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>a syphilis</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>includinghurricanes,floods,anddroughts</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>What is the aim of the Paris Agreement?</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Internationalagreements,suchastheParisAgreement,aimtolimitglobalwarming,butprogresshas beenslow.Publicawarenessandactivismaregrowing,withmovementscallingforstrongerpoliciesto addresstheclimatecrisis.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>['aimtolimitglobalwarming', 'to protect the interests of the people']</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>aimtolimitglobalwarming</t>
         </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>to protect the interests of the people</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>aimtolimitglobalwarming</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>